<commit_message>
Update STRD Dwelling StructurE_HIED HouseholdEquivalisedIncome_FMCFFamily Composition_VIC_20061116_IMAPconventionV2.xlsx
</commit_message>
<xml_diff>
--- a/assesmentData/STRD Dwelling StructurE_HIED HouseholdEquivalisedIncome_FMCFFamily Composition_VIC_20061116_IMAPconventionV2.xlsx
+++ b/assesmentData/STRD Dwelling StructurE_HIED HouseholdEquivalisedIncome_FMCFFamily Composition_VIC_20061116_IMAPconventionV2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\gr4sp\experiments\assesmentData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B1803D-0EDC-4482-8DF4-278656D9635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006EFD07-7624-4831-A8A5-0EC093F7C39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="38700" windowHeight="15435" xr2:uid="{9CA7CC69-ACCA-4866-9B50-D6BF25A9B8C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{9CA7CC69-ACCA-4866-9B50-D6BF25A9B8C4}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
@@ -645,8 +645,8 @@
   <dimension ref="A1:Z543"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A393" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F414" sqref="F414"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD66" sqref="AD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>